<commit_message>
Refactor log forwarder for sanitization and structure
Introduced a new log_sanitiser function to prepare for sanitizing logs and converting them to JSON. Updated file handling logic to use split_file helper and improved error handling. Added pseudo-code for a more robust log forwarder workflow, including privacy redaction and duplicate checks. Plan for moving forward is to use through different log files to detect which type (system, network etc), match each element of the log to its corresponding header (which differs between log types) and turn to json. Then will work out sanitizing and encryption.
</commit_message>
<xml_diff>
--- a/Designs/DatabaseDesign/FirestoreSchema.xlsx
+++ b/Designs/DatabaseDesign/FirestoreSchema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Github\Year3\COMP3000-Computing-Project\Designs\DatabaseDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C421B36-80DE-40A6-9B91-C3B43A68CBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F40DEBD-29C8-4C2B-8675-85A8120A4DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39495" yWindow="2880" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,38 @@
     <t>Fields:</t>
   </si>
   <si>
+    <t>processing_queue</t>
+  </si>
+  <si>
+    <t>Auto-generated UID</t>
+  </si>
+  <si>
+    <t>Handles the "circuit breaker" and "Async" logic for uploaded files. Backend puts the jobs here; frontend watches the status.</t>
+  </si>
+  <si>
+    <t>audit_logs</t>
+  </si>
+  <si>
+    <t>Record of who did what</t>
+  </si>
+  <si>
+    <t>file_name: og_001.json,
+ upload_timestamp: Timestamp,
+ status: processing, // Options: pending, processing, completed, failed
+error_message: null, // Populated if parsing fails [Error Handling]
+ user_id: user_uid</t>
+  </si>
+  <si>
+    <t>actor_id: user_uid",
+action: resolved_incident, // or "deleted_log", exported_report
+ target_resource_id: incident_id,
+ timestamp: Timestamp,
+ metadata: { previous_status: new, new_status: resolved }</t>
+  </si>
+  <si>
     <t xml:space="preserve">status: open, // Options: open, investigating, resolved [FR15]
 severity: high, // Options: low, medium, high, critical [FR10]
-timestamp_detected: "imestamp,
+timestamp_detected: timestamp,
 source_ip: 192.168.1.50,
 attack_type: Brute Force, // Extracted by Parser
 summary: "Multiple failed login attempts detected...", // [FR6] From LLM
@@ -90,35 +119,6 @@
  raw_log_reference: C://bucket_name/logs/file_123.log", // Traceability
 assigned_to: user_uid // Optional
 </t>
-  </si>
-  <si>
-    <t>processing_queue</t>
-  </si>
-  <si>
-    <t>Auto-generated UID</t>
-  </si>
-  <si>
-    <t>Handles the "circuit breaker" and "Async" logic for uploaded files. Backend puts the jobs here; frontend watches the status.</t>
-  </si>
-  <si>
-    <t>audit_logs</t>
-  </si>
-  <si>
-    <t>Record of who did what</t>
-  </si>
-  <si>
-    <t>file_name: og_001.json,
- upload_timestamp: Timestamp,
- status: processing, // Options: pending, processing, completed, failed
-error_message: null, // Populated if parsing fails [Error Handling]
- user_id: user_uid</t>
-  </si>
-  <si>
-    <t>actor_id: user_uid",
-action: resolved_incident, // or "deleted_log", exported_report
- target_resource_id: incident_id,
- timestamp: Timestamp,
- metadata: { previous_status: new, new_status: resolved }</t>
   </si>
 </sst>
 </file>
@@ -177,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -190,9 +190,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +495,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -512,7 +509,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -526,7 +523,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -540,7 +537,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -553,8 +550,8 @@
       <c r="E7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>18</v>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -568,7 +565,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -581,8 +578,8 @@
       <c r="E9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>16</v>
+      <c r="F9" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="189" customHeight="1" x14ac:dyDescent="0.3">
@@ -590,13 +587,13 @@
         <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>